<commit_message>
Updated segmentation parameters, as well as data and images
</commit_message>
<xml_diff>
--- a/Data/data_IHPC.png.xlsx
+++ b/Data/data_IHPC.png.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,32 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t>Grain Number</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Circumference</t>
-  </si>
-  <si>
-    <t>Area/Circumference</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Diameter</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -371,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,674 +353,665 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Grain Number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Circumference</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Area/Circumference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Width</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Diameter</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>37945</v>
+        <v>38051</v>
       </c>
       <c r="C2" t="n">
-        <v>2543</v>
+        <v>2513</v>
       </c>
       <c r="D2" t="n">
-        <v>14.92135273299253</v>
+        <v>15.141663350577</v>
       </c>
       <c r="E2" t="n">
-        <v>202.648193359375</v>
+        <v>203.715087890625</v>
       </c>
       <c r="F2" t="n">
-        <v>341.5977783203125</v>
+        <v>340.3763732910156</v>
       </c>
       <c r="G2" t="n">
-        <v>272.1229858398438</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>272.0457305908203</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="n">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>129999</v>
+        <v>130924</v>
       </c>
       <c r="C3" t="n">
-        <v>4956</v>
+        <v>5081</v>
       </c>
       <c r="D3" t="n">
-        <v>26.23062953995158</v>
+        <v>25.76736862822279</v>
       </c>
       <c r="E3" t="n">
-        <v>193.1249237060547</v>
+        <v>190.7676696777344</v>
       </c>
       <c r="F3" t="n">
-        <v>1087.227661132812</v>
+        <v>1093.575927734375</v>
       </c>
       <c r="G3" t="n">
-        <v>640.1762924194336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>642.1717987060547</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="n">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>14060</v>
+        <v>14074</v>
       </c>
       <c r="C4" t="n">
-        <v>1005</v>
+        <v>1018</v>
       </c>
       <c r="D4" t="n">
-        <v>13.99004975124378</v>
+        <v>13.82514734774067</v>
       </c>
       <c r="E4" t="n">
-        <v>91.29899597167969</v>
+        <v>91.38002014160156</v>
       </c>
       <c r="F4" t="n">
-        <v>226.5588531494141</v>
+        <v>226.1535186767578</v>
       </c>
       <c r="G4" t="n">
-        <v>158.9289245605469</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>158.7667694091797</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="n">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>54559</v>
+        <v>53582</v>
       </c>
       <c r="C5" t="n">
-        <v>2497</v>
+        <v>2398</v>
       </c>
       <c r="D5" t="n">
-        <v>21.84981978374049</v>
+        <v>22.34445371142619</v>
       </c>
       <c r="E5" t="n">
-        <v>180.3791351318359</v>
+        <v>164.7742767333984</v>
       </c>
       <c r="F5" t="n">
-        <v>443.5294799804688</v>
+        <v>446.3612670898438</v>
       </c>
       <c r="G5" t="n">
-        <v>311.9543075561523</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>305.5677719116211</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="n">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>7672</v>
+        <v>15746</v>
       </c>
       <c r="C6" t="n">
-        <v>607</v>
+        <v>1107</v>
       </c>
       <c r="D6" t="n">
-        <v>12.63920922570017</v>
+        <v>14.22402890695574</v>
       </c>
       <c r="E6" t="n">
-        <v>84.98950958251953</v>
+        <v>76.0003662109375</v>
       </c>
       <c r="F6" t="n">
-        <v>144.4574584960938</v>
+        <v>304.1217651367188</v>
       </c>
       <c r="G6" t="n">
-        <v>114.7234840393066</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>190.0610656738281</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="n">
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>45010</v>
+        <v>7730</v>
       </c>
       <c r="C7" t="n">
-        <v>2205</v>
+        <v>605</v>
       </c>
       <c r="D7" t="n">
-        <v>20.41269841269841</v>
+        <v>12.77685950413223</v>
       </c>
       <c r="E7" t="n">
-        <v>110.4207611083984</v>
+        <v>84.69525909423828</v>
       </c>
       <c r="F7" t="n">
-        <v>729.954833984375</v>
+        <v>144.7789001464844</v>
       </c>
       <c r="G7" t="n">
-        <v>420.1877975463867</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>114.7370796203613</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="n">
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>121459</v>
+        <v>43527</v>
       </c>
       <c r="C8" t="n">
-        <v>3112</v>
+        <v>2219</v>
       </c>
       <c r="D8" t="n">
-        <v>39.02924164524421</v>
+        <v>19.61559260928346</v>
       </c>
       <c r="E8" t="n">
-        <v>152.5390319824219</v>
+        <v>110.394775390625</v>
       </c>
       <c r="F8" t="n">
-        <v>1134.206909179688</v>
+        <v>731.8309936523438</v>
       </c>
       <c r="G8" t="n">
-        <v>643.3729705810547</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>421.1128845214844</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="n">
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>15832</v>
+        <v>123817</v>
       </c>
       <c r="C9" t="n">
-        <v>1121</v>
+        <v>3407</v>
       </c>
       <c r="D9" t="n">
-        <v>14.12310437109723</v>
+        <v>36.34194305840916</v>
       </c>
       <c r="E9" t="n">
-        <v>78.11688232421875</v>
+        <v>163.0025177001953</v>
       </c>
       <c r="F9" t="n">
-        <v>298.5306701660156</v>
+        <v>1096.718627929688</v>
       </c>
       <c r="G9" t="n">
-        <v>188.3237762451172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>629.8605728149414</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="n">
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>11028</v>
+        <v>11015</v>
       </c>
       <c r="C10" t="n">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D10" t="n">
-        <v>14.88259109311741</v>
+        <v>14.88513513513514</v>
       </c>
       <c r="E10" t="n">
-        <v>95.36217498779297</v>
+        <v>94.96884155273438</v>
       </c>
       <c r="F10" t="n">
-        <v>173.5040740966797</v>
+        <v>174.8611602783203</v>
       </c>
       <c r="G10" t="n">
-        <v>134.4331245422363</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>134.9150009155273</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="n">
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>28036</v>
+        <v>27891</v>
       </c>
       <c r="C11" t="n">
-        <v>1859</v>
+        <v>1825</v>
       </c>
       <c r="D11" t="n">
-        <v>15.08122646584185</v>
+        <v>15.2827397260274</v>
       </c>
       <c r="E11" t="n">
-        <v>92.18795776367188</v>
+        <v>89.30683135986328</v>
       </c>
       <c r="F11" t="n">
-        <v>463.4416809082031</v>
+        <v>469.91162109375</v>
       </c>
       <c r="G11" t="n">
-        <v>277.8148193359375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>279.6092262268066</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="n">
         <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>23452</v>
+        <v>23459</v>
       </c>
       <c r="C12" t="n">
-        <v>1767</v>
+        <v>1716</v>
       </c>
       <c r="D12" t="n">
-        <v>13.27221279003962</v>
+        <v>13.67074592074592</v>
       </c>
       <c r="E12" t="n">
-        <v>108.9104461669922</v>
+        <v>102.0355529785156</v>
       </c>
       <c r="F12" t="n">
-        <v>358.1949157714844</v>
+        <v>363.1114807128906</v>
       </c>
       <c r="G12" t="n">
-        <v>233.5526809692383</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>232.5735168457031</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="n">
         <v>17</v>
       </c>
       <c r="B13" t="n">
-        <v>131128</v>
+        <v>131722</v>
       </c>
       <c r="C13" t="n">
-        <v>6204</v>
+        <v>5921</v>
       </c>
       <c r="D13" t="n">
-        <v>21.13604126370084</v>
+        <v>22.24657996959973</v>
       </c>
       <c r="E13" t="n">
-        <v>250.8209991455078</v>
+        <v>251.8739929199219</v>
       </c>
       <c r="F13" t="n">
-        <v>854.48974609375</v>
+        <v>872.5260620117188</v>
       </c>
       <c r="G13" t="n">
-        <v>552.6553726196289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>562.2000274658203</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="n">
-        <v>70130</v>
+        <v>72503</v>
       </c>
       <c r="C14" t="n">
-        <v>5669</v>
+        <v>5536</v>
       </c>
       <c r="D14" t="n">
-        <v>12.37078849885341</v>
+        <v>13.0966401734104</v>
       </c>
       <c r="E14" t="n">
-        <v>292.4694213867188</v>
+        <v>290.5841369628906</v>
       </c>
       <c r="F14" t="n">
-        <v>754.3617553710938</v>
+        <v>745.5386962890625</v>
       </c>
       <c r="G14" t="n">
-        <v>523.4155883789062</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>518.0614166259766</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>9958</v>
+        <v>13453</v>
       </c>
       <c r="C15" t="n">
-        <v>967</v>
+        <v>1230</v>
       </c>
       <c r="D15" t="n">
-        <v>10.29782833505688</v>
+        <v>10.93739837398374</v>
       </c>
       <c r="E15" t="n">
-        <v>61.19269561767578</v>
+        <v>69.51529693603516</v>
       </c>
       <c r="F15" t="n">
-        <v>247.0439300537109</v>
+        <v>295.3503723144531</v>
       </c>
       <c r="G15" t="n">
-        <v>154.1183128356934</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>182.4328346252441</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>21109</v>
+        <v>21350</v>
       </c>
       <c r="C16" t="n">
-        <v>1429</v>
+        <v>1504</v>
       </c>
       <c r="D16" t="n">
-        <v>14.77186843946816</v>
+        <v>14.19547872340426</v>
       </c>
       <c r="E16" t="n">
-        <v>100.7132720947266</v>
+        <v>101.6572418212891</v>
       </c>
       <c r="F16" t="n">
-        <v>332.16162109375</v>
+        <v>327.8633117675781</v>
       </c>
       <c r="G16" t="n">
-        <v>216.4374465942383</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>214.7602767944336</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" t="n">
-        <v>88949</v>
+        <v>95884</v>
       </c>
       <c r="C17" t="n">
-        <v>5005</v>
+        <v>5192</v>
       </c>
       <c r="D17" t="n">
-        <v>17.77202797202797</v>
+        <v>18.46764252696456</v>
       </c>
       <c r="E17" t="n">
-        <v>301.4547729492188</v>
+        <v>303.9426574707031</v>
       </c>
       <c r="F17" t="n">
-        <v>673.9403686523438</v>
+        <v>678.7755126953125</v>
       </c>
       <c r="G17" t="n">
-        <v>487.6975708007812</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>491.3590850830078</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" t="n">
-        <v>9330</v>
+        <v>9296</v>
       </c>
       <c r="C18" t="n">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="D18" t="n">
-        <v>12.92243767313019</v>
+        <v>13.01960784313725</v>
       </c>
       <c r="E18" t="n">
-        <v>57.81745910644531</v>
+        <v>57.71804809570312</v>
       </c>
       <c r="F18" t="n">
-        <v>208.9766387939453</v>
+        <v>207.7810516357422</v>
       </c>
       <c r="G18" t="n">
-        <v>133.3970489501953</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>132.7495498657227</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="n">
+        <v>35</v>
+      </c>
+      <c r="B19" t="n">
+        <v>14790</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1216</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12.16282894736842</v>
+      </c>
+      <c r="E19" t="n">
+        <v>111.2822570800781</v>
+      </c>
+      <c r="F19" t="n">
+        <v>224.3874053955078</v>
+      </c>
+      <c r="G19" t="n">
+        <v>167.834831237793</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>36</v>
       </c>
-      <c r="B19" t="n">
-        <v>13946</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1252</v>
-      </c>
-      <c r="D19" t="n">
-        <v>11.13897763578275</v>
-      </c>
-      <c r="E19" t="n">
-        <v>94.77536773681641</v>
-      </c>
-      <c r="F19" t="n">
-        <v>238.8673553466797</v>
-      </c>
-      <c r="G19" t="n">
-        <v>166.821361541748</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="n">
-        <v>37</v>
-      </c>
       <c r="B20" t="n">
-        <v>20752</v>
+        <v>21024</v>
       </c>
       <c r="C20" t="n">
-        <v>1447</v>
+        <v>1470</v>
       </c>
       <c r="D20" t="n">
-        <v>14.34139599170698</v>
+        <v>14.30204081632653</v>
       </c>
       <c r="E20" t="n">
-        <v>68.07964324951172</v>
+        <v>67.62834167480469</v>
       </c>
       <c r="F20" t="n">
-        <v>456.0140991210938</v>
+        <v>472.8134460449219</v>
       </c>
       <c r="G20" t="n">
-        <v>262.0468711853027</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>270.2208938598633</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="n">
         <v>38</v>
       </c>
       <c r="B21" t="n">
-        <v>20992</v>
+        <v>20107</v>
       </c>
       <c r="C21" t="n">
-        <v>1338</v>
+        <v>1281</v>
       </c>
       <c r="D21" t="n">
-        <v>15.68908819133034</v>
+        <v>15.69633099141296</v>
       </c>
       <c r="E21" t="n">
-        <v>72.21625518798828</v>
+        <v>72.21975708007812</v>
       </c>
       <c r="F21" t="n">
-        <v>395.3281555175781</v>
+        <v>374.4579162597656</v>
       </c>
       <c r="G21" t="n">
-        <v>233.7722053527832</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>223.3388366699219</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="n">
         <v>39</v>
       </c>
       <c r="B22" t="n">
-        <v>7699</v>
+        <v>7959</v>
       </c>
       <c r="C22" t="n">
-        <v>720</v>
+        <v>780</v>
       </c>
       <c r="D22" t="n">
-        <v>10.69305555555556</v>
+        <v>10.20384615384615</v>
       </c>
       <c r="E22" t="n">
-        <v>84.42345428466797</v>
+        <v>80.21492004394531</v>
       </c>
       <c r="F22" t="n">
-        <v>140.9832000732422</v>
+        <v>142.5420837402344</v>
       </c>
       <c r="G22" t="n">
-        <v>112.7033271789551</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>111.3785018920898</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="n">
-        <v>26644</v>
+        <v>26796</v>
       </c>
       <c r="C23" t="n">
-        <v>1168</v>
+        <v>1229</v>
       </c>
       <c r="D23" t="n">
-        <v>22.81164383561644</v>
+        <v>21.80309194467046</v>
       </c>
       <c r="E23" t="n">
-        <v>99.14014434814453</v>
+        <v>98.70399475097656</v>
       </c>
       <c r="F23" t="n">
-        <v>391.6891784667969</v>
+        <v>409.5879821777344</v>
       </c>
       <c r="G23" t="n">
-        <v>245.4146614074707</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>254.1459884643555</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" t="n">
         <v>45</v>
       </c>
       <c r="B24" t="n">
-        <v>8329</v>
+        <v>26119</v>
       </c>
       <c r="C24" t="n">
-        <v>824</v>
+        <v>2182</v>
       </c>
       <c r="D24" t="n">
-        <v>10.10800970873786</v>
+        <v>11.97021081576535</v>
       </c>
       <c r="E24" t="n">
-        <v>82.38529205322266</v>
+        <v>153.1402282714844</v>
       </c>
       <c r="F24" t="n">
-        <v>168.3983459472656</v>
+        <v>334.2513122558594</v>
       </c>
       <c r="G24" t="n">
-        <v>125.3918190002441</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>243.6957702636719</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B25" t="n">
-        <v>22163</v>
+        <v>22336</v>
       </c>
       <c r="C25" t="n">
-        <v>1061</v>
+        <v>1088</v>
       </c>
       <c r="D25" t="n">
-        <v>20.88878416588124</v>
+        <v>20.52941176470588</v>
       </c>
       <c r="E25" t="n">
-        <v>105.9143829345703</v>
+        <v>106.2123870849609</v>
       </c>
       <c r="F25" t="n">
-        <v>306.1229248046875</v>
+        <v>311.486572265625</v>
       </c>
       <c r="G25" t="n">
-        <v>206.0186538696289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>208.849479675293</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B26" t="n">
-        <v>19259</v>
+        <v>16489</v>
       </c>
       <c r="C26" t="n">
-        <v>1621</v>
+        <v>701</v>
       </c>
       <c r="D26" t="n">
-        <v>11.88093769278223</v>
+        <v>23.52211126961484</v>
       </c>
       <c r="E26" t="n">
-        <v>161.6994934082031</v>
+        <v>111.766227722168</v>
       </c>
       <c r="F26" t="n">
-        <v>247.3382873535156</v>
+        <v>220.6231536865234</v>
       </c>
       <c r="G26" t="n">
-        <v>204.5188903808594</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>166.1946907043457</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B27" t="n">
-        <v>8462</v>
+        <v>7830</v>
       </c>
       <c r="C27" t="n">
-        <v>624</v>
+        <v>396</v>
       </c>
       <c r="D27" t="n">
-        <v>13.56089743589744</v>
+        <v>19.77272727272727</v>
       </c>
       <c r="E27" t="n">
-        <v>58.21109008789062</v>
+        <v>50.92024993896484</v>
       </c>
       <c r="F27" t="n">
-        <v>219.3460998535156</v>
+        <v>203.8961334228516</v>
       </c>
       <c r="G27" t="n">
-        <v>138.7785949707031</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>127.4081916809082</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" t="n">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B28" t="n">
-        <v>16325</v>
+        <v>8217</v>
       </c>
       <c r="C28" t="n">
-        <v>720</v>
+        <v>581</v>
       </c>
       <c r="D28" t="n">
-        <v>22.67361111111111</v>
+        <v>14.14285714285714</v>
       </c>
       <c r="E28" t="n">
-        <v>112.1910552978516</v>
+        <v>58.86418914794922</v>
       </c>
       <c r="F28" t="n">
-        <v>218.0421905517578</v>
+        <v>210.0706176757812</v>
       </c>
       <c r="G28" t="n">
-        <v>165.1166229248047</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="n">
-        <v>58</v>
-      </c>
-      <c r="B29" t="n">
-        <v>7631</v>
-      </c>
-      <c r="C29" t="n">
-        <v>413</v>
-      </c>
-      <c r="D29" t="n">
-        <v>18.47699757869249</v>
-      </c>
-      <c r="E29" t="n">
-        <v>50.81861114501953</v>
-      </c>
-      <c r="F29" t="n">
-        <v>200.8401031494141</v>
-      </c>
-      <c r="G29" t="n">
-        <v>125.8293571472168</v>
+        <v>134.4674034118652</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>